<commit_message>
Added settings page where you can manipulate the config file with dynamic data from dataframes.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -632,6 +632,132 @@
         <v>762.5</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CH-S09FTXF-NG</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>610</v>
+      </c>
+      <c r="D16" t="n">
+        <v>762.5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CH-S12FTXF-NG</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>661</v>
+      </c>
+      <c r="E17" t="n">
+        <v>826.25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CH-S09FTXF-NG</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>610</v>
+      </c>
+      <c r="C18" t="n">
+        <v>762.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CH-S12FTXF-NG</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>661</v>
+      </c>
+      <c r="C19" t="n">
+        <v>826.25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CH-S18FTXF-NG</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>950</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1187.5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CH-S09FTXF-NG</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1408</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CH-S18FTXLA2-NG</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>724</v>
+      </c>
+      <c r="C22" t="n">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CH-S12FTXLA2-NG</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>790</v>
+      </c>
+      <c r="C23" t="n">
+        <v>987.5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CH-S24FTXLA2-NG</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1269</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1586.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>